<commit_message>
saving Excel scripts w/ expression data
</commit_message>
<xml_diff>
--- a/test_scripts/all_bins_RNA/RNA_bins_normalized.xlsx
+++ b/test_scripts/all_bins_RNA/RNA_bins_normalized.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dgalambos/Documents/GitHub/meta-omics/test_scripts/all_bins_RNA/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A5A610-8FE0-7147-984A-835E750FC323}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="16100" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="21460" windowHeight="16020" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bin_by_bin_meancov_excelPrep" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">normalized!$A$1:$J$57</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -262,7 +263,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -400,6 +401,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -667,7 +671,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView topLeftCell="D19" workbookViewId="0">
@@ -2518,7 +2522,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -4861,13 +4865,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J57"/>
+  <autoFilter ref="A1:J57" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J120"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>